<commit_message>
adding my census data to the mix
</commit_message>
<xml_diff>
--- a/Gautham_Code/All_States_Census_Data.xlsx
+++ b/Gautham_Code/All_States_Census_Data.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gautham/Documents/CS506/CS506_Project/Gautham_Code/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189958B5-E558-A449-87F9-518516A10827}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="1780" yWindow="2280" windowWidth="33000" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All States" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -58,9 +64,6 @@
     <t>Hispanic (%)</t>
   </si>
   <si>
-    <t>White</t>
-  </si>
-  <si>
     <t>AL</t>
   </si>
   <si>
@@ -212,13 +215,16 @@
   </si>
   <si>
     <t>WY</t>
+  </si>
+  <si>
+    <t>White (%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,6 +287,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -327,7 +341,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -359,9 +373,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -393,6 +425,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -568,14 +618,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S52" sqref="S52"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -619,18 +671,18 @@
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" t="s">
-        <v>15</v>
       </c>
       <c r="B2">
         <v>4874747</v>
       </c>
       <c r="C2">
-        <v>94.40000000000001</v>
+        <v>94.4</v>
       </c>
       <c r="D2">
         <v>84.8</v>
@@ -645,7 +697,7 @@
         <v>24736</v>
       </c>
       <c r="H2">
-        <v>17.1</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="I2">
         <v>26.8</v>
@@ -669,9 +721,9 @@
         <v>65.8</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>739795</v>
@@ -716,9 +768,9 @@
         <v>61.2</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>7016270</v>
@@ -739,10 +791,10 @@
         <v>26686</v>
       </c>
       <c r="H4">
-        <v>16.4</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="I4">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="J4">
         <v>5.4</v>
@@ -763,9 +815,9 @@
         <v>55.5</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>3004279</v>
@@ -807,12 +859,12 @@
         <v>7.3</v>
       </c>
       <c r="O5">
-        <v>72.90000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+        <v>72.900000000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>39536653</v>
@@ -821,7 +873,7 @@
         <v>239.1</v>
       </c>
       <c r="D6">
-        <v>82.09999999999999</v>
+        <v>82.1</v>
       </c>
       <c r="E6">
         <v>32</v>
@@ -854,12 +906,12 @@
         <v>38.9</v>
       </c>
       <c r="O6">
-        <v>37.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7">
         <v>5607154</v>
@@ -871,7 +923,7 @@
         <v>91</v>
       </c>
       <c r="E7">
-        <v>38.7</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="F7">
         <v>62520</v>
@@ -901,12 +953,12 @@
         <v>21.3</v>
       </c>
       <c r="O7">
-        <v>68.59999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+        <v>68.599999999999994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8">
         <v>3588184</v>
@@ -915,7 +967,7 @@
         <v>738.1</v>
       </c>
       <c r="D8">
-        <v>90.09999999999999</v>
+        <v>90.1</v>
       </c>
       <c r="E8">
         <v>38</v>
@@ -927,7 +979,7 @@
         <v>39906</v>
       </c>
       <c r="H8">
-        <v>9.800000000000001</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="I8">
         <v>11.8</v>
@@ -942,7 +994,7 @@
         <v>0.1</v>
       </c>
       <c r="M8">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="N8">
         <v>15.7</v>
@@ -951,9 +1003,9 @@
         <v>67.7</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>693972</v>
@@ -974,7 +1026,7 @@
         <v>48781</v>
       </c>
       <c r="H9">
-        <v>18.6</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="I9">
         <v>47.7</v>
@@ -983,7 +1035,7 @@
         <v>0.6</v>
       </c>
       <c r="K9">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="L9">
         <v>0.2</v>
@@ -998,9 +1050,9 @@
         <v>36.4</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>961939</v>
@@ -1039,15 +1091,15 @@
         <v>2.6</v>
       </c>
       <c r="N10">
-        <v>9.199999999999999</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="O10">
         <v>62.9</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11">
         <v>20984400</v>
@@ -1092,9 +1144,9 @@
         <v>54.9</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12">
         <v>10429379</v>
@@ -1124,7 +1176,7 @@
         <v>0.5</v>
       </c>
       <c r="K12">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="L12">
         <v>0.1</v>
@@ -1139,9 +1191,9 @@
         <v>53.4</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13">
         <v>1427538</v>
@@ -1162,19 +1214,19 @@
         <v>30970</v>
       </c>
       <c r="H13">
-        <v>9.300000000000001</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="I13">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="J13">
         <v>0.4</v>
       </c>
       <c r="K13">
-        <v>37.7</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="L13">
-        <v>10.2</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="M13">
         <v>23.7</v>
@@ -1186,9 +1238,9 @@
         <v>22.1</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14">
         <v>1716943</v>
@@ -1230,12 +1282,12 @@
         <v>12.3</v>
       </c>
       <c r="O14">
-        <v>82.40000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
+        <v>82.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15">
         <v>12802023</v>
@@ -1280,9 +1332,9 @@
         <v>61.7</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16">
         <v>6666818</v>
@@ -1291,7 +1343,7 @@
         <v>181</v>
       </c>
       <c r="D16">
-        <v>88.09999999999999</v>
+        <v>88.1</v>
       </c>
       <c r="E16">
         <v>24.6</v>
@@ -1306,13 +1358,13 @@
         <v>14.1</v>
       </c>
       <c r="I16">
-        <v>9.699999999999999</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="J16">
         <v>0.4</v>
       </c>
       <c r="K16">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="L16">
         <v>0.1</v>
@@ -1324,12 +1376,12 @@
         <v>6.8</v>
       </c>
       <c r="O16">
-        <v>79.59999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
+        <v>79.599999999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17">
         <v>3145711</v>
@@ -1374,9 +1426,9 @@
         <v>86.2</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18">
         <v>2913123</v>
@@ -1421,9 +1473,9 @@
         <v>76.3</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19">
         <v>4454189</v>
@@ -1432,7 +1484,7 @@
         <v>109.9</v>
       </c>
       <c r="D19">
-        <v>84.59999999999999</v>
+        <v>84.6</v>
       </c>
       <c r="E19">
         <v>22.7</v>
@@ -1447,7 +1499,7 @@
         <v>18.5</v>
       </c>
       <c r="I19">
-        <v>8.300000000000001</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="J19">
         <v>0.3</v>
@@ -1468,9 +1520,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20">
         <v>4684333</v>
@@ -1515,9 +1567,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21">
         <v>1335907</v>
@@ -1526,7 +1578,7 @@
         <v>43.1</v>
       </c>
       <c r="D21">
-        <v>91.90000000000001</v>
+        <v>91.9</v>
       </c>
       <c r="E21">
         <v>29.3</v>
@@ -1550,27 +1602,30 @@
         <v>1.2</v>
       </c>
       <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
         <v>1.7</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>1.6</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <v>93.5</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22">
         <v>6052177</v>
       </c>
       <c r="C22">
-        <v>594.8</v>
+        <v>594.79999999999995</v>
       </c>
       <c r="D22">
-        <v>89.59999999999999</v>
+        <v>89.6</v>
       </c>
       <c r="E22">
         <v>38.4</v>
@@ -1582,7 +1637,7 @@
         <v>37756</v>
       </c>
       <c r="H22">
-        <v>9.699999999999999</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="I22">
         <v>30.7</v>
@@ -1600,15 +1655,15 @@
         <v>2.8</v>
       </c>
       <c r="N22">
-        <v>9.800000000000001</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="O22">
         <v>51.5</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23">
         <v>6859819</v>
@@ -1617,7 +1672,7 @@
         <v>839.4</v>
       </c>
       <c r="D23">
-        <v>90.09999999999999</v>
+        <v>90.1</v>
       </c>
       <c r="E23">
         <v>41.2</v>
@@ -1644,7 +1699,7 @@
         <v>0.1</v>
       </c>
       <c r="M23">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="N23">
         <v>11.5</v>
@@ -1653,9 +1708,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24">
         <v>9962311</v>
@@ -1664,7 +1719,7 @@
         <v>174.8</v>
       </c>
       <c r="D24">
-        <v>89.90000000000001</v>
+        <v>89.9</v>
       </c>
       <c r="E24">
         <v>27.4</v>
@@ -1688,30 +1743,33 @@
         <v>3.1</v>
       </c>
       <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
         <v>2.4</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>5</v>
       </c>
-      <c r="N24">
-        <v>75.40000000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="O24">
+        <v>75.400000000000006</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25">
         <v>5576606</v>
       </c>
       <c r="C25">
-        <v>66.59999999999999</v>
+        <v>66.599999999999994</v>
       </c>
       <c r="D25">
-        <v>92.59999999999999</v>
+        <v>92.6</v>
       </c>
       <c r="E25">
-        <v>34.2</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="F25">
         <v>63217</v>
@@ -1729,7 +1787,7 @@
         <v>1.3</v>
       </c>
       <c r="K25">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="L25">
         <v>0.1</v>
@@ -1741,12 +1799,12 @@
         <v>5.2</v>
       </c>
       <c r="O25">
-        <v>80.59999999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15">
+        <v>80.599999999999994</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26">
         <v>2984100</v>
@@ -1770,13 +1828,13 @@
         <v>20.8</v>
       </c>
       <c r="I26">
-        <v>37.7</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="J26">
         <v>0.6</v>
       </c>
       <c r="K26">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="L26">
         <v>0.1</v>
@@ -1791,15 +1849,15 @@
         <v>56.9</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27">
         <v>6113532</v>
       </c>
       <c r="C27">
-        <v>87.09999999999999</v>
+        <v>87.1</v>
       </c>
       <c r="D27">
         <v>88.8</v>
@@ -1829,18 +1887,18 @@
         <v>0.1</v>
       </c>
       <c r="M27">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="N27">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="O27">
         <v>79.7</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28">
         <v>1050493</v>
@@ -1849,7 +1907,7 @@
         <v>6.8</v>
       </c>
       <c r="D28">
-        <v>92.90000000000001</v>
+        <v>92.9</v>
       </c>
       <c r="E28">
         <v>29.9</v>
@@ -1885,9 +1943,9 @@
         <v>86.5</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29">
         <v>1920076</v>
@@ -1929,12 +1987,12 @@
         <v>10.7</v>
       </c>
       <c r="O29">
-        <v>79.59999999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15">
+        <v>79.599999999999994</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30">
         <v>2998039</v>
@@ -1943,7 +2001,7 @@
         <v>24.6</v>
       </c>
       <c r="D30">
-        <v>85.40000000000001</v>
+        <v>85.4</v>
       </c>
       <c r="E30">
         <v>23.2</v>
@@ -1964,7 +2022,7 @@
         <v>1.6</v>
       </c>
       <c r="K30">
-        <v>8.699999999999999</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="L30">
         <v>0.8</v>
@@ -1979,9 +2037,9 @@
         <v>49.9</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31">
         <v>1342795</v>
@@ -1990,7 +2048,7 @@
         <v>147</v>
       </c>
       <c r="D31">
-        <v>92.59999999999999</v>
+        <v>92.6</v>
       </c>
       <c r="E31">
         <v>35.5</v>
@@ -2026,9 +2084,9 @@
         <v>90.8</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B32">
         <v>9005644</v>
@@ -2037,7 +2095,7 @@
         <v>1195.5</v>
       </c>
       <c r="D32">
-        <v>88.90000000000001</v>
+        <v>88.9</v>
       </c>
       <c r="E32">
         <v>37.5</v>
@@ -2058,13 +2116,13 @@
         <v>0.6</v>
       </c>
       <c r="K32">
-        <v>9.800000000000001</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="L32">
         <v>0.1</v>
       </c>
       <c r="M32">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="N32">
         <v>20</v>
@@ -2073,9 +2131,9 @@
         <v>55.8</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33">
         <v>2088070</v>
@@ -2084,7 +2142,7 @@
         <v>17</v>
       </c>
       <c r="D33">
-        <v>84.59999999999999</v>
+        <v>84.6</v>
       </c>
       <c r="E33">
         <v>26.7</v>
@@ -2120,9 +2178,9 @@
         <v>38.1</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B34">
         <v>19849399</v>
@@ -2131,10 +2189,10 @@
         <v>411.2</v>
       </c>
       <c r="D34">
-        <v>85.90000000000001</v>
+        <v>85.9</v>
       </c>
       <c r="E34">
-        <v>34.7</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="F34">
         <v>60741</v>
@@ -2167,9 +2225,9 @@
         <v>55.8</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35">
         <v>10273419</v>
@@ -2205,24 +2263,24 @@
         <v>0.1</v>
       </c>
       <c r="M35">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="N35">
-        <v>9.199999999999999</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="O35">
         <v>63.5</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B36">
         <v>755393</v>
       </c>
       <c r="C36">
-        <v>9.699999999999999</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="D36">
         <v>92</v>
@@ -2261,9 +2319,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B37">
         <v>11658609</v>
@@ -2293,13 +2351,13 @@
         <v>0.3</v>
       </c>
       <c r="K37">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="L37">
         <v>0.1</v>
       </c>
       <c r="M37">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="N37">
         <v>3.7</v>
@@ -2308,9 +2366,9 @@
         <v>79.5</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B38">
         <v>3930864</v>
@@ -2337,10 +2395,10 @@
         <v>7.8</v>
       </c>
       <c r="J38">
-        <v>9.199999999999999</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="K38">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="L38">
         <v>0.2</v>
@@ -2355,9 +2413,9 @@
         <v>66.2</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B39">
         <v>4142776</v>
@@ -2399,18 +2457,18 @@
         <v>12.8</v>
       </c>
       <c r="O39">
-        <v>76.40000000000001</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15">
+        <v>76.400000000000006</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B40">
         <v>12805537</v>
       </c>
       <c r="C40">
-        <v>283.9</v>
+        <v>283.89999999999998</v>
       </c>
       <c r="D40">
         <v>89.5</v>
@@ -2449,9 +2507,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B41">
         <v>1059639</v>
@@ -2496,9 +2554,9 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B42">
         <v>5024369</v>
@@ -2543,9 +2601,9 @@
         <v>63.9</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B43">
         <v>869666</v>
@@ -2581,7 +2639,7 @@
         <v>0.1</v>
       </c>
       <c r="M43">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="N43">
         <v>3.7</v>
@@ -2590,9 +2648,9 @@
         <v>82.5</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B44">
         <v>6715984</v>
@@ -2616,7 +2674,7 @@
         <v>15.8</v>
       </c>
       <c r="I44">
-        <v>17.1</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="J44">
         <v>0.4</v>
@@ -2637,9 +2695,9 @@
         <v>74.2</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B45">
         <v>28304596</v>
@@ -2684,9 +2742,9 @@
         <v>42.6</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B46">
         <v>3101833</v>
@@ -2707,7 +2765,7 @@
         <v>25600</v>
       </c>
       <c r="H46">
-        <v>10.2</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="I46">
         <v>1.4</v>
@@ -2731,21 +2789,21 @@
         <v>78.8</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B47">
         <v>623657</v>
       </c>
       <c r="C47">
-        <v>67.90000000000001</v>
+        <v>67.900000000000006</v>
       </c>
       <c r="D47">
-        <v>91.90000000000001</v>
+        <v>91.9</v>
       </c>
       <c r="E47">
-        <v>36.2</v>
+        <v>36.200000000000003</v>
       </c>
       <c r="F47">
         <v>56104</v>
@@ -2766,18 +2824,21 @@
         <v>1.8</v>
       </c>
       <c r="L47">
-        <v>1.9</v>
+        <v>0</v>
       </c>
       <c r="M47">
         <v>1.9</v>
       </c>
       <c r="N47">
-        <v>93.09999999999999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15">
+        <v>1.9</v>
+      </c>
+      <c r="O47">
+        <v>93.1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B48">
         <v>8470020</v>
@@ -2786,7 +2847,7 @@
         <v>202.6</v>
       </c>
       <c r="D48">
-        <v>88.59999999999999</v>
+        <v>88.6</v>
       </c>
       <c r="E48">
         <v>36.9</v>
@@ -2822,9 +2883,9 @@
         <v>62.4</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B49">
         <v>7405743</v>
@@ -2833,7 +2894,7 @@
         <v>101.2</v>
       </c>
       <c r="D49">
-        <v>90.59999999999999</v>
+        <v>90.6</v>
       </c>
       <c r="E49">
         <v>33.6</v>
@@ -2848,7 +2909,7 @@
         <v>11.3</v>
       </c>
       <c r="I49">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="J49">
         <v>1.9</v>
@@ -2860,7 +2921,7 @@
         <v>0.8</v>
       </c>
       <c r="M49">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="N49">
         <v>12.4</v>
@@ -2869,21 +2930,21 @@
         <v>69.5</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B50">
         <v>1815857</v>
       </c>
       <c r="C50">
-        <v>77.09999999999999</v>
+        <v>77.099999999999994</v>
       </c>
       <c r="D50">
         <v>85.3</v>
       </c>
       <c r="E50">
-        <v>19.6</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="F50">
         <v>42644</v>
@@ -2892,7 +2953,7 @@
         <v>24002</v>
       </c>
       <c r="H50">
-        <v>17.9</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="I50">
         <v>3.6</v>
@@ -2904,18 +2965,21 @@
         <v>0.8</v>
       </c>
       <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
         <v>1.7</v>
       </c>
-      <c r="M50">
+      <c r="N50">
         <v>1.5</v>
       </c>
-      <c r="N50">
+      <c r="O50">
         <v>92.3</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B51">
         <v>5795483</v>
@@ -2924,7 +2988,7 @@
         <v>105</v>
       </c>
       <c r="D51">
-        <v>91.40000000000001</v>
+        <v>91.4</v>
       </c>
       <c r="E51">
         <v>28.4</v>
@@ -2942,7 +3006,7 @@
         <v>6.6</v>
       </c>
       <c r="J51">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K51">
         <v>2.8</v>
@@ -2960,9 +3024,9 @@
         <v>81.7</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B52">
         <v>579315</v>
@@ -2971,7 +3035,7 @@
         <v>5.8</v>
       </c>
       <c r="D52">
-        <v>92.40000000000001</v>
+        <v>92.4</v>
       </c>
       <c r="E52">
         <v>26</v>
@@ -3004,7 +3068,7 @@
         <v>10</v>
       </c>
       <c r="O52">
-        <v>84.09999999999999</v>
+        <v>84.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>